<commit_message>
Author          : Pranjal Kumar Singh Story Id        : SSDMS: 15, 21, 23,26 Files Modified  : PranjalSingh.xlsx Description     : Sprint Tracking Sheet modified for listing Tasks Breakdown. Reviewed by     : Ruchi Pareek
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
+++ b/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSDMS Project\Project\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranjal Kumar Singh\Desktop\SCGJ Project\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="SSDMS 15, 21, 23, 26" sheetId="6" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -82,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="51">
   <si>
     <t>Story ID</t>
   </si>
@@ -827,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -835,35 +838,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -893,21 +875,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -928,13 +910,65 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1214,35 +1248,35 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="67.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1256,296 +1290,300 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="30">
         <f>SUM(F2:F15)</f>
         <v>13.5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="11">
         <v>1.5</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11">
         <f>F2-G2</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="1:8" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="5">
+      <c r="F3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="4">
         <f>F3-G3</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="5">
+      <c r="F4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="4">
         <f t="shared" ref="H4:H26" si="0">F4-G4</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="5">
+      <c r="G5" s="12"/>
+      <c r="H5" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="5">
+      <c r="G6" s="12"/>
+      <c r="H6" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="5">
-        <v>2</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="5">
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="5">
-        <v>2</v>
-      </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="5">
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>1.5</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="5">
+      <c r="G9" s="12"/>
+      <c r="H9" s="4">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="5">
+      <c r="F10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="5">
+      <c r="G11" s="12"/>
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="5">
+      <c r="F12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="4">
         <f>F12-G12</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="11" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="5">
+      <c r="F13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="11" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="5">
+      <c r="F14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="5">
+      <c r="F15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -1557,733 +1595,733 @@
       <c r="G16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="7"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="3"/>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="35">
         <f>SUM(F18:F26)</f>
         <v>12</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <v>1.5</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="7">
+      <c r="G18" s="14"/>
+      <c r="H18" s="5">
         <f>F18-G18</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="13" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <v>1</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="7">
+      <c r="G19" s="14"/>
+      <c r="H19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="31"/>
+      <c r="B20" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="13" t="s">
+      <c r="C20" s="35"/>
+      <c r="D20" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7">
-        <v>2</v>
-      </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="7">
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="35"/>
+      <c r="D21" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="7">
-        <v>2</v>
-      </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="7">
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="13" t="s">
+      <c r="C22" s="35"/>
+      <c r="D22" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="7">
-        <v>2</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="7">
+      <c r="F22" s="5">
+        <v>2</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="31"/>
+      <c r="B23" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="13" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="7">
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="35"/>
+      <c r="D24" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="7">
+      <c r="F24" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="5">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="13" t="s">
+      <c r="C25" s="35"/>
+      <c r="D25" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="7">
+      <c r="F25" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="5">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="13" t="s">
+      <c r="C26" s="35"/>
+      <c r="D26" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="7">
+      <c r="F26" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="5">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="4"/>
+      <c r="B27" s="8"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="3"/>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="8"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="3"/>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="33">
         <f>SUM(F29:F42)</f>
         <v>13</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="35">
+      <c r="F29" s="25">
         <v>1.5</v>
       </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="9">
+      <c r="G29" s="15"/>
+      <c r="H29" s="6">
         <f t="shared" ref="H29:H36" si="1">F29-G29</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="15" t="s">
+      <c r="C30" s="33"/>
+      <c r="D30" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="9">
+      <c r="F30" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="15" t="s">
+      <c r="A31" s="34"/>
+      <c r="B31" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="15" t="s">
+      <c r="C31" s="33"/>
+      <c r="D31" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G31" s="22"/>
-      <c r="H31" s="9">
+      <c r="F31" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="15" t="s">
+      <c r="C32" s="33"/>
+      <c r="D32" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G32" s="22"/>
-      <c r="H32" s="9">
+      <c r="F32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="34"/>
+      <c r="B33" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="15" t="s">
+      <c r="C33" s="33"/>
+      <c r="D33" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="6">
         <v>1</v>
       </c>
-      <c r="G33" s="22"/>
-      <c r="H33" s="9">
+      <c r="G33" s="15"/>
+      <c r="H33" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="15" t="s">
+      <c r="A34" s="34"/>
+      <c r="B34" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="15" t="s">
+      <c r="C34" s="33"/>
+      <c r="D34" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="9">
-        <v>2</v>
-      </c>
-      <c r="G34" s="22"/>
-      <c r="H34" s="9">
+      <c r="F34" s="6">
+        <v>2</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="34"/>
+      <c r="B35" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="15" t="s">
+      <c r="C35" s="33"/>
+      <c r="D35" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="9">
-        <v>2</v>
-      </c>
-      <c r="G35" s="22"/>
-      <c r="H35" s="9">
+      <c r="F35" s="6">
+        <v>2</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="15" t="s">
+      <c r="C36" s="33"/>
+      <c r="D36" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36" s="6">
         <v>1.5</v>
       </c>
-      <c r="G36" s="22"/>
-      <c r="H36" s="9">
+      <c r="G36" s="15"/>
+      <c r="H36" s="6">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="34"/>
+      <c r="B37" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="15" t="s">
+      <c r="C37" s="33"/>
+      <c r="D37" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G37" s="22"/>
-      <c r="H37" s="9">
+      <c r="F37" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="6">
         <f>F40-G37</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="34"/>
+      <c r="B38" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="15" t="s">
+      <c r="C38" s="33"/>
+      <c r="D38" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="6">
         <v>1</v>
       </c>
-      <c r="G38" s="22"/>
-      <c r="H38" s="9">
+      <c r="G38" s="15"/>
+      <c r="H38" s="6">
         <f>F41-G38</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="34"/>
+      <c r="B39" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="15" t="s">
+      <c r="C39" s="33"/>
+      <c r="D39" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G39" s="22"/>
-      <c r="H39" s="9">
+      <c r="F39" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="15"/>
+      <c r="H39" s="6">
         <f>F42-G39</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="41"/>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="34"/>
+      <c r="B40" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="15" t="s">
+      <c r="C40" s="33"/>
+      <c r="D40" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G40" s="22"/>
-      <c r="H40" s="9">
+      <c r="F40" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="15"/>
+      <c r="H40" s="6">
         <f>F40-G40</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="34"/>
+      <c r="B41" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="D41" s="15" t="s">
+      <c r="C41" s="33"/>
+      <c r="D41" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G41" s="22"/>
-      <c r="H41" s="9">
+      <c r="F41" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="6">
         <f>F41-G41</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="34"/>
+      <c r="B42" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="15" t="s">
+      <c r="C42" s="33"/>
+      <c r="D42" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F42" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G42" s="22"/>
-      <c r="H42" s="9">
+      <c r="F42" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="15"/>
+      <c r="H42" s="6">
         <f>F42-G42</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
-      <c r="B43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="29"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="4"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="4"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="37">
+      <c r="C45" s="30">
         <f>SUM(F45:F53)</f>
         <v>12</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="34">
+      <c r="F45" s="24">
         <v>1.5</v>
       </c>
-      <c r="G45" s="19"/>
-      <c r="H45" s="5">
+      <c r="G45" s="12"/>
+      <c r="H45" s="4">
         <f t="shared" ref="H45:H53" si="2">F45-G45</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="39"/>
-      <c r="B46" s="11" t="s">
+      <c r="A46" s="32"/>
+      <c r="B46" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="11" t="s">
+      <c r="C46" s="30"/>
+      <c r="D46" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="24">
         <v>1</v>
       </c>
-      <c r="G46" s="19"/>
-      <c r="H46" s="5">
+      <c r="G46" s="12"/>
+      <c r="H46" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39"/>
-      <c r="B47" s="11" t="s">
+      <c r="A47" s="32"/>
+      <c r="B47" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="11" t="s">
+      <c r="C47" s="30"/>
+      <c r="D47" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="34">
-        <v>2</v>
-      </c>
-      <c r="G47" s="19"/>
-      <c r="H47" s="5">
+      <c r="F47" s="24">
+        <v>2</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="39"/>
-      <c r="B48" s="11" t="s">
+      <c r="A48" s="32"/>
+      <c r="B48" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="37"/>
-      <c r="D48" s="11" t="s">
+      <c r="C48" s="30"/>
+      <c r="D48" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E48" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F48" s="34">
-        <v>2</v>
-      </c>
-      <c r="G48" s="19"/>
-      <c r="H48" s="5">
+      <c r="F48" s="24">
+        <v>2</v>
+      </c>
+      <c r="G48" s="12"/>
+      <c r="H48" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="11" t="s">
+      <c r="A49" s="32"/>
+      <c r="B49" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="37"/>
-      <c r="D49" s="11" t="s">
+      <c r="C49" s="30"/>
+      <c r="D49" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="34">
-        <v>2</v>
-      </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="5">
+      <c r="F49" s="24">
+        <v>2</v>
+      </c>
+      <c r="G49" s="12"/>
+      <c r="H49" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="39"/>
-      <c r="B50" s="11" t="s">
+      <c r="A50" s="32"/>
+      <c r="B50" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="37"/>
-      <c r="D50" s="11" t="s">
+      <c r="C50" s="30"/>
+      <c r="D50" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="34">
-        <v>2</v>
-      </c>
-      <c r="G50" s="19"/>
-      <c r="H50" s="5">
+      <c r="F50" s="24">
+        <v>2</v>
+      </c>
+      <c r="G50" s="12"/>
+      <c r="H50" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="39"/>
-      <c r="B51" s="11" t="s">
+      <c r="A51" s="32"/>
+      <c r="B51" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="37"/>
-      <c r="D51" s="11" t="s">
+      <c r="C51" s="30"/>
+      <c r="D51" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="G51" s="19"/>
-      <c r="H51" s="5">
+      <c r="F51" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="4">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="39"/>
-      <c r="B52" s="11" t="s">
+      <c r="A52" s="32"/>
+      <c r="B52" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="37"/>
-      <c r="D52" s="11" t="s">
+      <c r="C52" s="30"/>
+      <c r="D52" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="G52" s="19"/>
-      <c r="H52" s="5">
+      <c r="F52" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="4">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="39"/>
-      <c r="B53" s="11" t="s">
+      <c r="A53" s="32"/>
+      <c r="B53" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="37"/>
-      <c r="D53" s="11" t="s">
+      <c r="C53" s="30"/>
+      <c r="D53" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F53" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="G53" s="19"/>
-      <c r="H53" s="5">
+      <c r="F53" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="4">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="25">
+      <c r="C54" s="18">
         <f>SUM(C2:C53)</f>
         <v>50.5</v>
       </c>
@@ -2303,8 +2341,8 @@
     <mergeCell ref="C18:C26"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Author          : Pranjal Kumar Singh Story Id        : SSDMS: 15, 21, 23,26 Files Modified  : PranjalSingh.xlsx Description     : Hours Burnt Updated.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
+++ b/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="58">
   <si>
     <t>Story ID</t>
   </si>
@@ -696,13 +696,16 @@
   </si>
   <si>
     <t>Understand backward &amp; Forward linkages</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,13 +730,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -905,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -990,9 +986,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1001,45 +994,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1054,6 +1008,55 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1365,10 +1368,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,9 +1383,10 @@
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
@@ -1407,15 +1411,18 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="I1" s="60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="51">
         <f>SUM(F2:F18)</f>
         <v>16</v>
       </c>
@@ -1435,13 +1442,16 @@
         <f>F2-G2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="I2" s="61">
+        <v>42801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
       <c r="B3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="45"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="32" t="s">
         <v>21</v>
       </c>
@@ -1458,13 +1468,14 @@
         <f t="shared" ref="H3:H4" si="0">F3-G3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="I3" s="61"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
       <c r="B4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="32" t="s">
         <v>22</v>
       </c>
@@ -1481,13 +1492,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="I4" s="61"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
       <c r="B5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="45"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="32" t="s">
         <v>23</v>
       </c>
@@ -1497,292 +1509,320 @@
       <c r="F5" s="35">
         <v>1.5</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="59">
+        <v>1.5</v>
+      </c>
       <c r="H5" s="35">
         <f>F5-G5</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="61">
+        <v>42832</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="49"/>
       <c r="B6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="28">
         <v>0.5</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="37">
+        <v>0.5</v>
+      </c>
       <c r="H6" s="28">
         <f>F6-G6</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="61"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
       <c r="B7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="45"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
         <v>42</v>
       </c>
       <c r="F7" s="28">
         <v>0.5</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="37">
+        <v>0.5</v>
+      </c>
       <c r="H7" s="28">
         <f t="shared" ref="H7:H32" si="1">F7-G7</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="61"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
       <c r="B8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="45"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="36" t="s">
         <v>43</v>
       </c>
       <c r="F8" s="28">
         <v>1</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="37">
+        <v>1</v>
+      </c>
       <c r="H8" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="61"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
       <c r="B9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="36" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="28">
         <v>1</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="37">
+        <v>1</v>
+      </c>
       <c r="H9" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="61"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
       <c r="B10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="28">
         <v>2</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="37">
+        <v>2</v>
+      </c>
       <c r="H10" s="28">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="61"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
       <c r="B11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="45"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="36" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="28">
         <v>2</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="28">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="I11" s="62"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
       <c r="B12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="45"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="36" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="28">
         <v>1.5</v>
       </c>
-      <c r="G12" s="38"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="28">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="I12" s="62"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
       <c r="B13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="45"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="36" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="28">
         <v>0.5</v>
       </c>
-      <c r="G13" s="38"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="28">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="I13" s="62"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="49"/>
       <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="45"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="36" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="28">
         <v>1</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="I14" s="62"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
       <c r="B15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="36" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="28">
         <v>0.5</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="28">
         <f>F15-G15</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="I15" s="62"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
       <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="36" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="28">
         <v>0.5</v>
       </c>
-      <c r="G16" s="38"/>
+      <c r="G16" s="37"/>
       <c r="H16" s="28">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="I16" s="62"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
       <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="36" t="s">
         <v>35</v>
       </c>
       <c r="F17" s="28">
         <v>0.5</v>
       </c>
-      <c r="G17" s="38"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="28">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="I17" s="62"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
       <c r="B18" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="36" t="s">
         <v>37</v>
       </c>
       <c r="F18" s="28">
         <v>0.5</v>
       </c>
-      <c r="G18" s="38"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="28">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="62"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
@@ -1790,291 +1830,303 @@
       <c r="F20" s="3"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="56">
         <f>SUM(F21:F32)</f>
         <v>14.5</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="55" t="s">
+      <c r="E21" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="56">
-        <v>1</v>
-      </c>
-      <c r="G21" s="56">
-        <v>1</v>
-      </c>
-      <c r="H21" s="56">
+      <c r="F21" s="42">
+        <v>1</v>
+      </c>
+      <c r="G21" s="42">
+        <v>1</v>
+      </c>
+      <c r="H21" s="42">
         <f>F21-G21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="53" t="s">
+      <c r="I21" s="64"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="54"/>
+      <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="53" t="s">
+      <c r="C22" s="56"/>
+      <c r="D22" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="56">
-        <v>1</v>
-      </c>
-      <c r="G22" s="56">
-        <v>1</v>
-      </c>
-      <c r="H22" s="56">
+      <c r="F22" s="42">
+        <v>1</v>
+      </c>
+      <c r="G22" s="42">
+        <v>1</v>
+      </c>
+      <c r="H22" s="42">
         <f t="shared" ref="H22:H23" si="2">F22-G22</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="53" t="s">
+      <c r="I22" s="64"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="54"/>
+      <c r="B23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="53" t="s">
+      <c r="C23" s="56"/>
+      <c r="D23" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="56">
-        <v>0.5</v>
-      </c>
-      <c r="G23" s="56">
-        <v>0.5</v>
-      </c>
-      <c r="H23" s="56">
+      <c r="F23" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="53" t="s">
+      <c r="I23" s="64"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="54"/>
+      <c r="B24" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="53" t="s">
+      <c r="C24" s="56"/>
+      <c r="D24" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="56">
+      <c r="F24" s="42">
         <v>1.5</v>
       </c>
-      <c r="G24" s="58"/>
-      <c r="H24" s="56">
+      <c r="G24" s="44"/>
+      <c r="H24" s="42">
         <f>F24-G24</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="53" t="s">
+      <c r="I24" s="64"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+      <c r="B25" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="53" t="s">
+      <c r="C25" s="56"/>
+      <c r="D25" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="56">
-        <v>1</v>
-      </c>
-      <c r="G25" s="58"/>
-      <c r="H25" s="56">
+      <c r="F25" s="42">
+        <v>1</v>
+      </c>
+      <c r="G25" s="44"/>
+      <c r="H25" s="42">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="53" t="s">
+      <c r="I25" s="64"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
+      <c r="B26" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="53" t="s">
+      <c r="C26" s="56"/>
+      <c r="D26" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="56">
+      <c r="F26" s="42">
         <v>2</v>
       </c>
-      <c r="G26" s="58"/>
-      <c r="H26" s="56">
+      <c r="G26" s="44"/>
+      <c r="H26" s="42">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="53" t="s">
+      <c r="I26" s="64"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="54"/>
+      <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="53" t="s">
+      <c r="C27" s="56"/>
+      <c r="D27" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="56">
+      <c r="F27" s="42">
         <v>2</v>
       </c>
-      <c r="G27" s="58"/>
-      <c r="H27" s="56">
+      <c r="G27" s="44"/>
+      <c r="H27" s="42">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="53" t="s">
+      <c r="I27" s="64"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="53" t="s">
+      <c r="C28" s="56"/>
+      <c r="D28" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="56">
+      <c r="F28" s="42">
         <v>2</v>
       </c>
-      <c r="G28" s="58"/>
-      <c r="H28" s="56">
+      <c r="G28" s="44"/>
+      <c r="H28" s="42">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="53" t="s">
+      <c r="I28" s="64"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
+      <c r="B29" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="53" t="s">
+      <c r="C29" s="56"/>
+      <c r="D29" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="56">
+      <c r="F29" s="42">
         <v>2</v>
       </c>
-      <c r="G29" s="58"/>
-      <c r="H29" s="56">
+      <c r="G29" s="44"/>
+      <c r="H29" s="42">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="53" t="s">
+      <c r="I29" s="64"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+      <c r="B30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="53" t="s">
+      <c r="C30" s="56"/>
+      <c r="D30" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="59" t="s">
+      <c r="E30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="56">
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="58"/>
-      <c r="H30" s="56">
+      <c r="F30" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="44"/>
+      <c r="H30" s="42">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="53" t="s">
+      <c r="I30" s="64"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="53" t="s">
+      <c r="C31" s="56"/>
+      <c r="D31" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="56">
-        <v>0.5</v>
-      </c>
-      <c r="G31" s="58"/>
-      <c r="H31" s="56">
+      <c r="F31" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="44"/>
+      <c r="H31" s="42">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="53" t="s">
+      <c r="I31" s="64"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="55"/>
+      <c r="B32" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="53" t="s">
+      <c r="C32" s="56"/>
+      <c r="D32" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="56">
-        <v>0.5</v>
-      </c>
-      <c r="G32" s="58"/>
-      <c r="H32" s="56">
+      <c r="F32" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="44"/>
+      <c r="H32" s="42">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="64"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="D33" s="3"/>
       <c r="E33" s="11"/>
       <c r="F33" s="3"/>
       <c r="G33"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="D34" s="3"/>
       <c r="E34" s="11"/>
       <c r="F34" s="3"/>
       <c r="G34"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="58">
         <f>SUM(F35:F51)</f>
         <v>15.5</v>
       </c>
@@ -2094,13 +2146,14 @@
         <f>F35-G35</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
+      <c r="I35" s="63"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="57"/>
       <c r="B36" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="50"/>
+      <c r="C36" s="58"/>
       <c r="D36" s="19" t="s">
         <v>21</v>
       </c>
@@ -2117,13 +2170,14 @@
         <f>F36-G36</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
+      <c r="I36" s="63"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="57"/>
       <c r="B37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="50"/>
+      <c r="C37" s="58"/>
       <c r="D37" s="19" t="s">
         <v>22</v>
       </c>
@@ -2140,13 +2194,14 @@
         <f>F37-G37</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
+      <c r="I37" s="63"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="57"/>
       <c r="B38" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="50"/>
+      <c r="C38" s="58"/>
       <c r="D38" s="19" t="s">
         <v>23</v>
       </c>
@@ -2161,13 +2216,14 @@
         <f t="shared" ref="H38:H45" si="3">F38-G38</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
+      <c r="I38" s="63"/>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="57"/>
       <c r="B39" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="50"/>
+      <c r="C39" s="58"/>
       <c r="D39" s="19" t="s">
         <v>24</v>
       </c>
@@ -2182,13 +2238,14 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
+      <c r="I39" s="63"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="57"/>
       <c r="B40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="50"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="19" t="s">
         <v>25</v>
       </c>
@@ -2203,13 +2260,14 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
+      <c r="I40" s="63"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="57"/>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="50"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="19" t="s">
         <v>26</v>
       </c>
@@ -2224,13 +2282,14 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
+      <c r="I41" s="63"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="57"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="50"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="19" t="s">
         <v>27</v>
       </c>
@@ -2245,13 +2304,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
+      <c r="I42" s="63"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="57"/>
       <c r="B43" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="50"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2266,13 +2326,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
+      <c r="I43" s="63"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="57"/>
       <c r="B44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="50"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
@@ -2287,13 +2348,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
+      <c r="I44" s="63"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="57"/>
       <c r="B45" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="50"/>
+      <c r="C45" s="58"/>
       <c r="D45" s="19" t="s">
         <v>36</v>
       </c>
@@ -2308,13 +2370,14 @@
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
+      <c r="I45" s="63"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
       <c r="B46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="50"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="19" t="s">
         <v>38</v>
       </c>
@@ -2329,13 +2392,14 @@
         <f>F49-G46</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
+      <c r="I46" s="63"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="57"/>
       <c r="B47" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="50"/>
+      <c r="C47" s="58"/>
       <c r="D47" s="19" t="s">
         <v>44</v>
       </c>
@@ -2350,13 +2414,14 @@
         <f>F50-G47</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="49"/>
+      <c r="I47" s="63"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="57"/>
       <c r="B48" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="50"/>
+      <c r="C48" s="58"/>
       <c r="D48" s="19" t="s">
         <v>45</v>
       </c>
@@ -2371,13 +2436,14 @@
         <f>F51-G48</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="49"/>
+      <c r="I48" s="63"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="57"/>
       <c r="B49" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="50"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="19" t="s">
         <v>52</v>
       </c>
@@ -2392,13 +2458,14 @@
         <f>F49-G49</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="49"/>
+      <c r="I49" s="63"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="57"/>
       <c r="B50" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="50"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2413,13 +2480,14 @@
         <f>F50-G50</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="49"/>
+      <c r="I50" s="63"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="57"/>
       <c r="B51" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="50"/>
+      <c r="C51" s="58"/>
       <c r="D51" s="19" t="s">
         <v>54</v>
       </c>
@@ -2434,8 +2502,9 @@
         <f>F51-G51</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="63"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="15"/>
       <c r="D52" s="15"/>
@@ -2444,7 +2513,7 @@
       <c r="G52" s="18"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="15"/>
       <c r="D53" s="15"/>
@@ -2453,14 +2522,14 @@
       <c r="G53" s="18"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="51" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="52">
+      <c r="C54" s="47">
         <f>SUM(F54:F65)</f>
         <v>14.5</v>
       </c>
@@ -2481,12 +2550,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="51"/>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="46"/>
       <c r="B55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="52"/>
+      <c r="C55" s="47"/>
       <c r="D55" s="20" t="s">
         <v>21</v>
       </c>
@@ -2504,12 +2573,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="51"/>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="46"/>
       <c r="B56" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="52"/>
+      <c r="C56" s="47"/>
       <c r="D56" s="20" t="s">
         <v>22</v>
       </c>
@@ -2527,12 +2596,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="51"/>
+    <row r="57" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="46"/>
       <c r="B57" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="52"/>
+      <c r="C57" s="47"/>
       <c r="D57" s="20" t="s">
         <v>23</v>
       </c>
@@ -2548,12 +2617,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="51"/>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="46"/>
       <c r="B58" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="52"/>
+      <c r="C58" s="47"/>
       <c r="D58" s="20" t="s">
         <v>24</v>
       </c>
@@ -2569,12 +2638,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="51"/>
+    <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="46"/>
       <c r="B59" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="52"/>
+      <c r="C59" s="47"/>
       <c r="D59" s="20" t="s">
         <v>25</v>
       </c>
@@ -2590,12 +2659,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="51"/>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="46"/>
       <c r="B60" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="52"/>
+      <c r="C60" s="47"/>
       <c r="D60" s="20" t="s">
         <v>26</v>
       </c>
@@ -2611,12 +2680,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="51"/>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="46"/>
       <c r="B61" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="52"/>
+      <c r="C61" s="47"/>
       <c r="D61" s="20" t="s">
         <v>27</v>
       </c>
@@ -2632,12 +2701,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="51"/>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="46"/>
       <c r="B62" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="52"/>
+      <c r="C62" s="47"/>
       <c r="D62" s="20" t="s">
         <v>32</v>
       </c>
@@ -2653,12 +2722,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="51"/>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="46"/>
       <c r="B63" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="52"/>
+      <c r="C63" s="47"/>
       <c r="D63" s="20" t="s">
         <v>34</v>
       </c>
@@ -2674,12 +2743,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="51"/>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="46"/>
       <c r="B64" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="52"/>
+      <c r="C64" s="47"/>
       <c r="D64" s="20" t="s">
         <v>36</v>
       </c>
@@ -2696,11 +2765,11 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="51"/>
+      <c r="A65" s="46"/>
       <c r="B65" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="52"/>
+      <c r="C65" s="47"/>
       <c r="D65" s="20" t="s">
         <v>38</v>
       </c>
@@ -2717,10 +2786,10 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="39" t="s">
+      <c r="B66" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="40">
+      <c r="C66" s="39">
         <f>SUM(C2:C65)</f>
         <v>60.5</v>
       </c>
@@ -2729,7 +2798,9 @@
       <c r="G66"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I10"/>
     <mergeCell ref="A54:A65"/>
     <mergeCell ref="C54:C65"/>
     <mergeCell ref="A2:A18"/>

</xml_diff>

<commit_message>
Author          : Pranjal Kumar Singh Story Id        : SSDMS: 15, 21, 23, 26 Files Modified  : PranjalSingh.xlsx Description     : Hours Burnt Updated.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
+++ b/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranjal Kumar Singh\Desktop\SCGJ Project\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranjal Kumar Singh\Desktop\SCGJ\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="59">
   <si>
     <t>Story ID</t>
   </si>
@@ -699,6 +699,9 @@
   </si>
   <si>
     <t>Completion Date</t>
+  </si>
+  <si>
+    <t>Hours Needed</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +816,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1008,45 +1017,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1057,6 +1027,74 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,7 +1409,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1419,7 @@
     <col min="4" max="4" width="10.5703125" style="6" customWidth="1"/>
     <col min="5" max="5" width="67.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1411,18 +1449,18 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="47" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="58">
         <f>SUM(F2:F18)</f>
         <v>16</v>
       </c>
@@ -1442,16 +1480,16 @@
         <f>F2-G2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="61">
+      <c r="I2" s="52">
         <v>42801</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="52"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="32" t="s">
         <v>21</v>
       </c>
@@ -1468,14 +1506,14 @@
         <f t="shared" ref="H3:H4" si="0">F3-G3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="61"/>
+      <c r="I3" s="52"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="32" t="s">
         <v>22</v>
       </c>
@@ -1492,14 +1530,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I4" s="61"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="52"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="32" t="s">
         <v>23</v>
       </c>
@@ -1509,23 +1547,23 @@
       <c r="F5" s="35">
         <v>1.5</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="46">
         <v>1.5</v>
       </c>
       <c r="H5" s="35">
         <f>F5-G5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="61">
+      <c r="I5" s="66">
         <v>42832</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="52"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="32" t="s">
         <v>24</v>
       </c>
@@ -1542,14 +1580,14 @@
         <f>F6-G6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="61"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="52"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="32" t="s">
         <v>25</v>
       </c>
@@ -1566,14 +1604,14 @@
         <f t="shared" ref="H7:H32" si="1">F7-G7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="61"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="32" t="s">
         <v>26</v>
       </c>
@@ -1590,14 +1628,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="61"/>
+      <c r="I8" s="67"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="32" t="s">
         <v>27</v>
       </c>
@@ -1614,14 +1652,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="61"/>
+      <c r="I9" s="68"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="52"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="32" t="s">
         <v>32</v>
       </c>
@@ -1638,14 +1676,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="61"/>
+      <c r="I10" s="52">
+        <v>42862</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="52"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="32" t="s">
         <v>34</v>
       </c>
@@ -1655,19 +1695,21 @@
       <c r="F11" s="28">
         <v>2</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="37">
+        <v>2</v>
+      </c>
       <c r="H11" s="28">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I11" s="62"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="52"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="32" t="s">
         <v>36</v>
       </c>
@@ -1677,19 +1719,21 @@
       <c r="F12" s="28">
         <v>1.5</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="37">
+        <v>1.5</v>
+      </c>
       <c r="H12" s="28">
         <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="I12" s="62"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="32" t="s">
         <v>38</v>
       </c>
@@ -1704,14 +1748,14 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I13" s="62"/>
+      <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="52"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="32" t="s">
         <v>44</v>
       </c>
@@ -1721,19 +1765,23 @@
       <c r="F14" s="28">
         <v>1</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="37">
+        <v>1</v>
+      </c>
       <c r="H14" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="62"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="48">
+        <v>42862</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="52"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="32" t="s">
         <v>45</v>
       </c>
@@ -1748,14 +1796,14 @@
         <f>F15-G15</f>
         <v>0.5</v>
       </c>
-      <c r="I15" s="62"/>
+      <c r="I15" s="49"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="52"/>
+      <c r="C16" s="59"/>
       <c r="D16" s="32" t="s">
         <v>52</v>
       </c>
@@ -1770,14 +1818,14 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="49"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="52"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="32" t="s">
         <v>53</v>
       </c>
@@ -1792,14 +1840,14 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I17" s="62"/>
+      <c r="I17" s="49"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="53"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="32" t="s">
         <v>54</v>
       </c>
@@ -1814,13 +1862,19 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I18" s="62"/>
+      <c r="I18" s="49"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="D19"/>
       <c r="E19"/>
-      <c r="G19"/>
+      <c r="G19" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="75">
+        <f>SUM(H2:H18)</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -1831,13 +1885,13 @@
       <c r="G20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="63">
         <f>SUM(F21:F32)</f>
         <v>14.5</v>
       </c>
@@ -1857,14 +1911,14 @@
         <f>F21-G21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="64"/>
+      <c r="I21" s="51"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="56"/>
+      <c r="C22" s="63"/>
       <c r="D22" s="40" t="s">
         <v>21</v>
       </c>
@@ -1881,14 +1935,14 @@
         <f t="shared" ref="H22:H23" si="2">F22-G22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="64"/>
+      <c r="I22" s="51"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="40" t="s">
         <v>22</v>
       </c>
@@ -1905,14 +1959,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="64"/>
+      <c r="I23" s="51"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="56"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="40" t="s">
         <v>23</v>
       </c>
@@ -1927,14 +1981,14 @@
         <f>F24-G24</f>
         <v>1.5</v>
       </c>
-      <c r="I24" s="64"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="56"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="40" t="s">
         <v>24</v>
       </c>
@@ -1949,14 +2003,14 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I25" s="64"/>
+      <c r="I25" s="51"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="56"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="40" t="s">
         <v>25</v>
       </c>
@@ -1971,14 +2025,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I26" s="64"/>
+      <c r="I26" s="51"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="56"/>
+      <c r="C27" s="63"/>
       <c r="D27" s="40" t="s">
         <v>26</v>
       </c>
@@ -1993,14 +2047,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I27" s="64"/>
+      <c r="I27" s="51"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="56"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="40" t="s">
         <v>27</v>
       </c>
@@ -2015,14 +2069,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I28" s="64"/>
+      <c r="I28" s="51"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="56"/>
+      <c r="C29" s="63"/>
       <c r="D29" s="40" t="s">
         <v>32</v>
       </c>
@@ -2037,14 +2091,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I29" s="64"/>
+      <c r="I29" s="51"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="56"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="40" t="s">
         <v>34</v>
       </c>
@@ -2059,14 +2113,14 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I30" s="64"/>
+      <c r="I30" s="51"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="40" t="s">
         <v>36</v>
       </c>
@@ -2081,14 +2135,14 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I31" s="64"/>
+      <c r="I31" s="51"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="56"/>
+      <c r="C32" s="63"/>
       <c r="D32" s="40" t="s">
         <v>38</v>
       </c>
@@ -2103,14 +2157,20 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I32" s="64"/>
+      <c r="I32" s="51"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="D33" s="3"/>
       <c r="E33" s="11"/>
       <c r="F33" s="3"/>
-      <c r="G33"/>
+      <c r="G33" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="75">
+        <f>SUM(H21:H32)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
@@ -2120,13 +2180,13 @@
       <c r="G34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="64" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="58">
+      <c r="C35" s="65">
         <f>SUM(F35:F51)</f>
         <v>15.5</v>
       </c>
@@ -2146,14 +2206,16 @@
         <f>F35-G35</f>
         <v>0</v>
       </c>
-      <c r="I35" s="63"/>
+      <c r="I35" s="71">
+        <v>42801</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="57"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="65"/>
       <c r="D36" s="19" t="s">
         <v>21</v>
       </c>
@@ -2170,14 +2232,14 @@
         <f>F36-G36</f>
         <v>0</v>
       </c>
-      <c r="I36" s="63"/>
+      <c r="I36" s="72"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="57"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="65"/>
       <c r="D37" s="19" t="s">
         <v>22</v>
       </c>
@@ -2194,14 +2256,14 @@
         <f>F37-G37</f>
         <v>0</v>
       </c>
-      <c r="I37" s="63"/>
+      <c r="I37" s="73"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="57"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="58"/>
+      <c r="C38" s="65"/>
       <c r="D38" s="19" t="s">
         <v>23</v>
       </c>
@@ -2211,19 +2273,23 @@
       <c r="F38" s="9">
         <v>1.5</v>
       </c>
-      <c r="G38" s="10"/>
+      <c r="G38" s="10">
+        <v>1.5</v>
+      </c>
       <c r="H38" s="4">
         <f t="shared" ref="H38:H45" si="3">F38-G38</f>
-        <v>1.5</v>
-      </c>
-      <c r="I38" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="69">
+        <v>42862</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="58"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="19" t="s">
         <v>24</v>
       </c>
@@ -2233,19 +2299,21 @@
       <c r="F39" s="4">
         <v>0.5</v>
       </c>
-      <c r="G39" s="10"/>
+      <c r="G39" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H39" s="4">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="I39" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="69"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="57"/>
+      <c r="A40" s="64"/>
       <c r="B40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="58"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="19" t="s">
         <v>25</v>
       </c>
@@ -2255,19 +2323,21 @@
       <c r="F40" s="4">
         <v>0.5</v>
       </c>
-      <c r="G40" s="10"/>
+      <c r="G40" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H40" s="4">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="I40" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="69"/>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="57"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="58"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="19" t="s">
         <v>26</v>
       </c>
@@ -2277,19 +2347,21 @@
       <c r="F41" s="4">
         <v>0.5</v>
       </c>
-      <c r="G41" s="10"/>
+      <c r="G41" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H41" s="4">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="I41" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="69"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="57"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="58"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="19" t="s">
         <v>27</v>
       </c>
@@ -2299,19 +2371,21 @@
       <c r="F42" s="4">
         <v>1</v>
       </c>
-      <c r="G42" s="10"/>
+      <c r="G42" s="4">
+        <v>1</v>
+      </c>
       <c r="H42" s="4">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I42" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="69"/>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="58"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2321,19 +2395,21 @@
       <c r="F43" s="4">
         <v>2</v>
       </c>
-      <c r="G43" s="10"/>
+      <c r="G43" s="4">
+        <v>2</v>
+      </c>
       <c r="H43" s="4">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I43" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="69"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="58"/>
+      <c r="C44" s="65"/>
       <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
@@ -2343,19 +2419,21 @@
       <c r="F44" s="4">
         <v>2</v>
       </c>
-      <c r="G44" s="10"/>
+      <c r="G44" s="4">
+        <v>2</v>
+      </c>
       <c r="H44" s="4">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I44" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="69"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="58"/>
+      <c r="C45" s="65"/>
       <c r="D45" s="19" t="s">
         <v>36</v>
       </c>
@@ -2365,19 +2443,21 @@
       <c r="F45" s="4">
         <v>1.5</v>
       </c>
-      <c r="G45" s="10"/>
+      <c r="G45" s="4">
+        <v>1.5</v>
+      </c>
       <c r="H45" s="4">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="I45" s="63"/>
+        <f>F45-G45</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="69"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="58"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="19" t="s">
         <v>38</v>
       </c>
@@ -2389,17 +2469,17 @@
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="4">
-        <f>F49-G46</f>
-        <v>0.5</v>
-      </c>
-      <c r="I46" s="63"/>
+        <f t="shared" ref="H46:H51" si="4">F46-G46</f>
+        <v>0.5</v>
+      </c>
+      <c r="I46" s="50"/>
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="58"/>
+      <c r="C47" s="65"/>
       <c r="D47" s="19" t="s">
         <v>44</v>
       </c>
@@ -2409,19 +2489,23 @@
       <c r="F47" s="4">
         <v>1</v>
       </c>
-      <c r="G47" s="10"/>
+      <c r="G47" s="10">
+        <v>1</v>
+      </c>
       <c r="H47" s="4">
-        <f>F50-G47</f>
-        <v>0.5</v>
-      </c>
-      <c r="I47" s="63"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="70">
+        <v>42862</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="58"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="19" t="s">
         <v>45</v>
       </c>
@@ -2433,17 +2517,17 @@
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="4">
-        <f>F51-G48</f>
-        <v>0.5</v>
-      </c>
-      <c r="I48" s="63"/>
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="50"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="58"/>
+      <c r="C49" s="65"/>
       <c r="D49" s="19" t="s">
         <v>52</v>
       </c>
@@ -2455,17 +2539,17 @@
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="4">
-        <f>F49-G49</f>
-        <v>0.5</v>
-      </c>
-      <c r="I49" s="63"/>
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I49" s="50"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
+      <c r="A50" s="64"/>
       <c r="B50" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="58"/>
+      <c r="C50" s="65"/>
       <c r="D50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2477,17 +2561,17 @@
       </c>
       <c r="G50" s="10"/>
       <c r="H50" s="4">
-        <f>F50-G50</f>
-        <v>0.5</v>
-      </c>
-      <c r="I50" s="63"/>
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I50" s="50"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="58"/>
+      <c r="C51" s="65"/>
       <c r="D51" s="19" t="s">
         <v>54</v>
       </c>
@@ -2499,10 +2583,10 @@
       </c>
       <c r="G51" s="10"/>
       <c r="H51" s="4">
-        <f>F51-G51</f>
-        <v>0.5</v>
-      </c>
-      <c r="I51" s="63"/>
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="50"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
@@ -2510,8 +2594,13 @@
       <c r="D52" s="15"/>
       <c r="E52" s="16"/>
       <c r="F52" s="17"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="17"/>
+      <c r="G52" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="H52" s="75">
+        <f>SUM(H35:H51)</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
@@ -2523,13 +2612,13 @@
       <c r="H53" s="17"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="46" t="s">
+      <c r="A54" s="53" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="47">
+      <c r="C54" s="54">
         <f>SUM(F54:F65)</f>
         <v>14.5</v>
       </c>
@@ -2551,11 +2640,11 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="46"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="47"/>
+      <c r="C55" s="54"/>
       <c r="D55" s="20" t="s">
         <v>21</v>
       </c>
@@ -2574,11 +2663,11 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="46"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="47"/>
+      <c r="C56" s="54"/>
       <c r="D56" s="20" t="s">
         <v>22</v>
       </c>
@@ -2597,11 +2686,11 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="47"/>
+      <c r="C57" s="54"/>
       <c r="D57" s="20" t="s">
         <v>23</v>
       </c>
@@ -2613,16 +2702,16 @@
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="5">
-        <f t="shared" ref="H57:H65" si="4">F57-G57</f>
+        <f t="shared" ref="H57:H65" si="5">F57-G57</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="46"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="47"/>
+      <c r="C58" s="54"/>
       <c r="D58" s="20" t="s">
         <v>24</v>
       </c>
@@ -2634,16 +2723,16 @@
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="46"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="47"/>
+      <c r="C59" s="54"/>
       <c r="D59" s="20" t="s">
         <v>25</v>
       </c>
@@ -2655,16 +2744,16 @@
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="46"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="47"/>
+      <c r="C60" s="54"/>
       <c r="D60" s="20" t="s">
         <v>26</v>
       </c>
@@ -2676,16 +2765,16 @@
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="46"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="47"/>
+      <c r="C61" s="54"/>
       <c r="D61" s="20" t="s">
         <v>27</v>
       </c>
@@ -2697,16 +2786,16 @@
       </c>
       <c r="G61" s="12"/>
       <c r="H61" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="46"/>
+      <c r="A62" s="53"/>
       <c r="B62" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="47"/>
+      <c r="C62" s="54"/>
       <c r="D62" s="20" t="s">
         <v>32</v>
       </c>
@@ -2718,16 +2807,16 @@
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="46"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="47"/>
+      <c r="C63" s="54"/>
       <c r="D63" s="20" t="s">
         <v>34</v>
       </c>
@@ -2739,16 +2828,16 @@
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="46"/>
+      <c r="A64" s="53"/>
       <c r="B64" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="47"/>
+      <c r="C64" s="54"/>
       <c r="D64" s="20" t="s">
         <v>36</v>
       </c>
@@ -2760,16 +2849,16 @@
       </c>
       <c r="G64" s="12"/>
       <c r="H64" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="46"/>
+      <c r="A65" s="53"/>
       <c r="B65" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="47"/>
+      <c r="C65" s="54"/>
       <c r="D65" s="20" t="s">
         <v>38</v>
       </c>
@@ -2781,7 +2870,7 @@
       </c>
       <c r="G65" s="12"/>
       <c r="H65" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2795,12 +2884,17 @@
       </c>
       <c r="D66"/>
       <c r="E66"/>
-      <c r="G66"/>
+      <c r="G66" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="H66" s="75">
+        <f>SUM(H54:H65)</f>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
     <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I10"/>
     <mergeCell ref="A54:A65"/>
     <mergeCell ref="C54:C65"/>
     <mergeCell ref="A2:A18"/>
@@ -2809,6 +2903,10 @@
     <mergeCell ref="C21:C32"/>
     <mergeCell ref="A35:A51"/>
     <mergeCell ref="C35:C51"/>
+    <mergeCell ref="I5:I9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="I38:I45"/>
+    <mergeCell ref="I35:I37"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author          : Pranjal Kumar Singh Files Modified  : PranjalSingh.xlsx Description     : Burnt hours Updated
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
+++ b/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="64">
   <si>
     <t>Story ID</t>
   </si>
@@ -712,13 +712,40 @@
   </si>
   <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <r>
+      <t>Understand the existing code (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Created New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Hours Left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,6 +798,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -958,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1071,6 +1105,45 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1110,12 +1183,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,7 +1192,7 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,37 +1204,14 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1481,10 +1525,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1540,7 @@
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="77" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="56" customWidth="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1528,18 +1572,18 @@
       <c r="I1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="J1" s="52" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="67" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="57">
+      <c r="C2" s="70">
         <f>SUM(F2:F18)</f>
         <v>16</v>
       </c>
@@ -1559,19 +1603,19 @@
         <f>F2-G2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="66">
+      <c r="I2" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="64">
         <v>42801</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="68"/>
       <c r="B3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="32" t="s">
         <v>21</v>
       </c>
@@ -1588,17 +1632,17 @@
         <f t="shared" ref="H3:H4" si="0">F3-G3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="66"/>
+      <c r="I3" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="64"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="32" t="s">
         <v>22</v>
       </c>
@@ -1615,17 +1659,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I4" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="66"/>
+      <c r="I4" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="32" t="s">
         <v>23</v>
       </c>
@@ -1642,19 +1686,19 @@
         <f>F5-G5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="67">
+      <c r="I5" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="78">
         <v>42832</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="32" t="s">
         <v>24</v>
       </c>
@@ -1671,17 +1715,17 @@
         <f>F6-G6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="68"/>
+      <c r="I6" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="79"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="32" t="s">
         <v>25</v>
       </c>
@@ -1698,17 +1742,17 @@
         <f t="shared" ref="H7:H32" si="1">F7-G7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="68"/>
+      <c r="I7" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="79"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="32" t="s">
         <v>26</v>
       </c>
@@ -1725,17 +1769,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="68"/>
+      <c r="I8" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="79"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="32" t="s">
         <v>27</v>
       </c>
@@ -1752,17 +1796,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="69"/>
+      <c r="I9" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="80"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="32" t="s">
         <v>32</v>
       </c>
@@ -1779,19 +1823,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="66">
+      <c r="I10" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="64">
         <v>42862</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
+      <c r="A11" s="68"/>
       <c r="B11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="32" t="s">
         <v>34</v>
       </c>
@@ -1808,17 +1852,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="66"/>
+      <c r="I11" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="64"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="58"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="32" t="s">
         <v>36</v>
       </c>
@@ -1835,17 +1879,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="66"/>
+      <c r="I12" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="64"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="58"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="32" t="s">
         <v>38</v>
       </c>
@@ -1860,17 +1904,17 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="57" t="s">
         <v>61</v>
       </c>
       <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="58"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="32" t="s">
         <v>44</v>
       </c>
@@ -1887,19 +1931,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="70">
+      <c r="I14" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="53">
         <v>42862</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="32" t="s">
         <v>45</v>
       </c>
@@ -1914,17 +1958,17 @@
         <f>F15-G15</f>
         <v>0.5</v>
       </c>
-      <c r="I15" s="78" t="s">
+      <c r="I15" s="57" t="s">
         <v>61</v>
       </c>
       <c r="J15" s="47"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="32" t="s">
         <v>52</v>
       </c>
@@ -1939,17 +1983,17 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I16" s="78" t="s">
+      <c r="I16" s="57" t="s">
         <v>61</v>
       </c>
       <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
+      <c r="A17" s="68"/>
       <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="58"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="32" t="s">
         <v>53</v>
       </c>
@@ -1964,17 +2008,17 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I17" s="78" t="s">
+      <c r="I17" s="57" t="s">
         <v>61</v>
       </c>
       <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
+      <c r="A18" s="69"/>
       <c r="B18" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="59"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="32" t="s">
         <v>54</v>
       </c>
@@ -1989,7 +2033,7 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I18" s="78" t="s">
+      <c r="I18" s="57" t="s">
         <v>61</v>
       </c>
       <c r="J18" s="47"/>
@@ -2005,7 +2049,7 @@
         <f>SUM(H2:H18)</f>
         <v>2.5</v>
       </c>
-      <c r="I19" s="76"/>
+      <c r="I19" s="55"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -2016,13 +2060,13 @@
       <c r="G20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="73" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="62">
+      <c r="C21" s="75">
         <f>SUM(F21:F32)</f>
         <v>14.5</v>
       </c>
@@ -2042,17 +2086,19 @@
         <f>F21-G21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" s="49"/>
+      <c r="I21" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="85">
+        <v>42801</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="62"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="40" t="s">
         <v>21</v>
       </c>
@@ -2069,17 +2115,17 @@
         <f t="shared" ref="H22:H23" si="2">F22-G22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="49"/>
+      <c r="I22" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" s="75"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="60"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="62"/>
+      <c r="C23" s="75"/>
       <c r="D23" s="40" t="s">
         <v>22</v>
       </c>
@@ -2096,17 +2142,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" s="49"/>
+      <c r="I23" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="75"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="60"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="62"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="40" t="s">
         <v>23</v>
       </c>
@@ -2116,22 +2162,26 @@
       <c r="F24" s="42">
         <v>1.5</v>
       </c>
-      <c r="G24" s="44"/>
+      <c r="G24" s="44">
+        <v>1.5</v>
+      </c>
       <c r="H24" s="42">
         <f>F24-G24</f>
-        <v>1.5</v>
-      </c>
-      <c r="I24" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="J24" s="49"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24" s="85">
+        <v>42892</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
+      <c r="A25" s="73"/>
       <c r="B25" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="62"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="40" t="s">
         <v>24</v>
       </c>
@@ -2141,22 +2191,24 @@
       <c r="F25" s="42">
         <v>1</v>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="44">
+        <v>0.5</v>
+      </c>
       <c r="H25" s="42">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="49"/>
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" s="75"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="60"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="62"/>
+      <c r="C26" s="75"/>
       <c r="D26" s="40" t="s">
         <v>25</v>
       </c>
@@ -2166,22 +2218,24 @@
       <c r="F26" s="42">
         <v>2</v>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="44">
+        <v>1.5</v>
+      </c>
       <c r="H26" s="42">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I26" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="49"/>
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" s="75"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="60"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="62"/>
+      <c r="C27" s="75"/>
       <c r="D27" s="40" t="s">
         <v>26</v>
       </c>
@@ -2191,22 +2245,24 @@
       <c r="F27" s="42">
         <v>2</v>
       </c>
-      <c r="G27" s="44"/>
+      <c r="G27" s="44">
+        <v>1</v>
+      </c>
       <c r="H27" s="42">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I27" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="J27" s="49"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J27" s="75"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="60"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="62"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="40" t="s">
         <v>27</v>
       </c>
@@ -2216,22 +2272,24 @@
       <c r="F28" s="42">
         <v>2</v>
       </c>
-      <c r="G28" s="44"/>
+      <c r="G28" s="44">
+        <v>0.1</v>
+      </c>
       <c r="H28" s="42">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I28" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="J28" s="49"/>
+        <v>1.9</v>
+      </c>
+      <c r="I28" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" s="75"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="75"/>
       <c r="D29" s="40" t="s">
         <v>32</v>
       </c>
@@ -2241,22 +2299,24 @@
       <c r="F29" s="42">
         <v>2</v>
       </c>
-      <c r="G29" s="44"/>
+      <c r="G29" s="44">
+        <v>0.1</v>
+      </c>
       <c r="H29" s="42">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I29" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="J29" s="49"/>
+        <v>1.9</v>
+      </c>
+      <c r="I29" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="75"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="62"/>
+      <c r="C30" s="75"/>
       <c r="D30" s="40" t="s">
         <v>34</v>
       </c>
@@ -2271,17 +2331,17 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I30" s="82" t="s">
+      <c r="I30" s="61" t="s">
         <v>61</v>
       </c>
       <c r="J30" s="49"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="60"/>
+      <c r="A31" s="73"/>
       <c r="B31" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="75"/>
       <c r="D31" s="40" t="s">
         <v>36</v>
       </c>
@@ -2296,17 +2356,17 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I31" s="82" t="s">
+      <c r="I31" s="61" t="s">
         <v>61</v>
       </c>
       <c r="J31" s="49"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="62"/>
+      <c r="C32" s="75"/>
       <c r="D32" s="40" t="s">
         <v>38</v>
       </c>
@@ -2321,7 +2381,7 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I32" s="82" t="s">
+      <c r="I32" s="61" t="s">
         <v>61</v>
       </c>
       <c r="J32" s="49"/>
@@ -2336,9 +2396,9 @@
       </c>
       <c r="H33" s="51">
         <f>SUM(H21:H32)</f>
-        <v>12</v>
-      </c>
-      <c r="I33" s="76"/>
+        <v>7.3</v>
+      </c>
+      <c r="I33" s="55"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
@@ -2348,13 +2408,13 @@
       <c r="G34"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="76" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="64">
+      <c r="C35" s="77">
         <f>SUM(F35:F51)</f>
         <v>15.5</v>
       </c>
@@ -2374,19 +2434,19 @@
         <f>F35-G35</f>
         <v>0</v>
       </c>
-      <c r="I35" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J35" s="71">
+      <c r="I35" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J35" s="82">
         <v>42801</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="63"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="64"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="19" t="s">
         <v>21</v>
       </c>
@@ -2403,17 +2463,17 @@
         <f>F36-G36</f>
         <v>0</v>
       </c>
-      <c r="I36" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J36" s="72"/>
+      <c r="I36" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" s="83"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="63"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="64"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="19" t="s">
         <v>22</v>
       </c>
@@ -2430,17 +2490,17 @@
         <f>F37-G37</f>
         <v>0</v>
       </c>
-      <c r="I37" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J37" s="73"/>
+      <c r="I37" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" s="84"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="63"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="64"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="19" t="s">
         <v>23</v>
       </c>
@@ -2457,19 +2517,19 @@
         <f t="shared" ref="H38:H44" si="3">F38-G38</f>
         <v>1.4</v>
       </c>
-      <c r="I38" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J38" s="74">
+      <c r="I38" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J38" s="81">
         <v>42862</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="63"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="64"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="19" t="s">
         <v>24</v>
       </c>
@@ -2486,17 +2546,17 @@
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="I39" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J39" s="74"/>
+      <c r="I39" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J39" s="81"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="63"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="64"/>
+      <c r="C40" s="77"/>
       <c r="D40" s="19" t="s">
         <v>25</v>
       </c>
@@ -2513,17 +2573,17 @@
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="I40" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J40" s="74"/>
+      <c r="I40" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J40" s="81"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="63"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="64"/>
+      <c r="C41" s="77"/>
       <c r="D41" s="19" t="s">
         <v>26</v>
       </c>
@@ -2540,17 +2600,17 @@
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="I41" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J41" s="74"/>
+      <c r="I41" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J41" s="81"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="63"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="64"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="19" t="s">
         <v>27</v>
       </c>
@@ -2567,17 +2627,17 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="I42" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J42" s="74"/>
+      <c r="I42" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J42" s="81"/>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="63"/>
+      <c r="A43" s="76"/>
       <c r="B43" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="64"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2594,17 +2654,17 @@
         <f t="shared" si="3"/>
         <v>1.9</v>
       </c>
-      <c r="I43" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J43" s="74"/>
+      <c r="I43" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J43" s="81"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="63"/>
+      <c r="A44" s="76"/>
       <c r="B44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="64"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
@@ -2621,17 +2681,17 @@
         <f t="shared" si="3"/>
         <v>1.9</v>
       </c>
-      <c r="I44" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J44" s="74"/>
+      <c r="I44" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J44" s="81"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
+      <c r="A45" s="76"/>
       <c r="B45" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="64"/>
+      <c r="C45" s="77"/>
       <c r="D45" s="19" t="s">
         <v>36</v>
       </c>
@@ -2648,17 +2708,17 @@
         <f>F45-G45</f>
         <v>1.4</v>
       </c>
-      <c r="I45" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J45" s="74"/>
+      <c r="I45" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J45" s="81"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
+      <c r="A46" s="76"/>
       <c r="B46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="64"/>
+      <c r="C46" s="77"/>
       <c r="D46" s="19" t="s">
         <v>38</v>
       </c>
@@ -2673,17 +2733,17 @@
         <f t="shared" ref="H46:H51" si="4">F46-G46</f>
         <v>0.5</v>
       </c>
-      <c r="I46" s="83" t="s">
+      <c r="I46" s="62" t="s">
         <v>61</v>
       </c>
       <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="63"/>
+      <c r="A47" s="76"/>
       <c r="B47" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="64"/>
+      <c r="C47" s="77"/>
       <c r="D47" s="19" t="s">
         <v>44</v>
       </c>
@@ -2694,25 +2754,25 @@
         <v>1</v>
       </c>
       <c r="G47" s="10">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I47" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="J47" s="75">
+        <v>0.9</v>
+      </c>
+      <c r="I47" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J47" s="54">
         <v>42862</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="63"/>
+      <c r="A48" s="76"/>
       <c r="B48" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="64"/>
+      <c r="C48" s="77"/>
       <c r="D48" s="19" t="s">
         <v>45</v>
       </c>
@@ -2727,17 +2787,17 @@
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="I48" s="83" t="s">
+      <c r="I48" s="62" t="s">
         <v>61</v>
       </c>
       <c r="J48" s="48"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
+      <c r="A49" s="76"/>
       <c r="B49" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="64"/>
+      <c r="C49" s="77"/>
       <c r="D49" s="19" t="s">
         <v>52</v>
       </c>
@@ -2752,17 +2812,17 @@
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="I49" s="83" t="s">
+      <c r="I49" s="62" t="s">
         <v>61</v>
       </c>
       <c r="J49" s="48"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="63"/>
+      <c r="A50" s="76"/>
       <c r="B50" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="64"/>
+      <c r="C50" s="77"/>
       <c r="D50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2777,17 +2837,17 @@
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="I50" s="83" t="s">
+      <c r="I50" s="62" t="s">
         <v>61</v>
       </c>
       <c r="J50" s="48"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="63"/>
+      <c r="A51" s="76"/>
       <c r="B51" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="64"/>
+      <c r="C51" s="77"/>
       <c r="D51" s="19" t="s">
         <v>54</v>
       </c>
@@ -2802,7 +2862,7 @@
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="I51" s="83" t="s">
+      <c r="I51" s="62" t="s">
         <v>61</v>
       </c>
       <c r="J51" s="48"/>
@@ -2818,9 +2878,9 @@
       </c>
       <c r="H52" s="51">
         <f>SUM(H35:H51)</f>
-        <v>11.2</v>
-      </c>
-      <c r="I52" s="76"/>
+        <v>12.1</v>
+      </c>
+      <c r="I52" s="55"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
@@ -2830,16 +2890,16 @@
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
       <c r="H53" s="17"/>
-      <c r="I53" s="76"/>
+      <c r="I53" s="55"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="52" t="s">
+      <c r="A54" s="65" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="53">
+      <c r="C54" s="66">
         <f>SUM(F54:F65)</f>
         <v>14.5</v>
       </c>
@@ -2859,17 +2919,19 @@
         <f>F54-G54</f>
         <v>0</v>
       </c>
-      <c r="I54" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J54" s="49"/>
+      <c r="I54" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J54" s="86">
+        <v>42801</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="52"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="53"/>
+      <c r="C55" s="66"/>
       <c r="D55" s="20" t="s">
         <v>21</v>
       </c>
@@ -2886,17 +2948,17 @@
         <f>F55-G55</f>
         <v>0</v>
       </c>
-      <c r="I55" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J55" s="49"/>
+      <c r="I55" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J55" s="66"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="53"/>
+      <c r="C56" s="66"/>
       <c r="D56" s="20" t="s">
         <v>22</v>
       </c>
@@ -2913,42 +2975,46 @@
         <f>F56-G56</f>
         <v>0</v>
       </c>
-      <c r="I56" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J56" s="49"/>
+      <c r="I56" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J56" s="66"/>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="52"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="53"/>
+      <c r="C57" s="66"/>
       <c r="D57" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F57" s="31">
         <v>1.5</v>
       </c>
-      <c r="G57" s="12"/>
+      <c r="G57" s="12">
+        <v>1.5</v>
+      </c>
       <c r="H57" s="5">
         <f t="shared" ref="H57:H65" si="5">F57-G57</f>
-        <v>1.5</v>
-      </c>
-      <c r="I57" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J57" s="49"/>
+        <v>0</v>
+      </c>
+      <c r="I57" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J57" s="86">
+        <v>42892</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="53"/>
+      <c r="C58" s="66"/>
       <c r="D58" s="20" t="s">
         <v>24</v>
       </c>
@@ -2958,22 +3024,24 @@
       <c r="F58" s="31">
         <v>1</v>
       </c>
-      <c r="G58" s="12"/>
+      <c r="G58" s="12">
+        <v>0.1</v>
+      </c>
       <c r="H58" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="I58" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J58" s="49"/>
+        <v>0.9</v>
+      </c>
+      <c r="I58" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J58" s="66"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="52"/>
+      <c r="A59" s="65"/>
       <c r="B59" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="53"/>
+      <c r="C59" s="66"/>
       <c r="D59" s="20" t="s">
         <v>25</v>
       </c>
@@ -2983,22 +3051,24 @@
       <c r="F59" s="31">
         <v>2</v>
       </c>
-      <c r="G59" s="12"/>
+      <c r="G59" s="12">
+        <v>1.5</v>
+      </c>
       <c r="H59" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I59" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J59" s="49"/>
+        <v>0.5</v>
+      </c>
+      <c r="I59" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J59" s="66"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="52"/>
+      <c r="A60" s="65"/>
       <c r="B60" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="53"/>
+      <c r="C60" s="66"/>
       <c r="D60" s="20" t="s">
         <v>26</v>
       </c>
@@ -3008,22 +3078,24 @@
       <c r="F60" s="31">
         <v>2</v>
       </c>
-      <c r="G60" s="12"/>
+      <c r="G60" s="12">
+        <v>0.1</v>
+      </c>
       <c r="H60" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I60" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J60" s="49"/>
+        <v>1.9</v>
+      </c>
+      <c r="I60" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="66"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
+      <c r="A61" s="65"/>
       <c r="B61" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="53"/>
+      <c r="C61" s="66"/>
       <c r="D61" s="20" t="s">
         <v>27</v>
       </c>
@@ -3033,22 +3105,24 @@
       <c r="F61" s="31">
         <v>2</v>
       </c>
-      <c r="G61" s="12"/>
+      <c r="G61" s="12">
+        <v>0.1</v>
+      </c>
       <c r="H61" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I61" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J61" s="49"/>
+        <v>1.9</v>
+      </c>
+      <c r="I61" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61" s="66"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="52"/>
+      <c r="A62" s="65"/>
       <c r="B62" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="53"/>
+      <c r="C62" s="66"/>
       <c r="D62" s="20" t="s">
         <v>32</v>
       </c>
@@ -3058,22 +3132,24 @@
       <c r="F62" s="31">
         <v>2</v>
       </c>
-      <c r="G62" s="12"/>
+      <c r="G62" s="12">
+        <v>0.1</v>
+      </c>
       <c r="H62" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I62" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="J62" s="49"/>
+        <v>1.9</v>
+      </c>
+      <c r="I62" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J62" s="66"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="52"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="53"/>
+      <c r="C63" s="66"/>
       <c r="D63" s="20" t="s">
         <v>34</v>
       </c>
@@ -3088,17 +3164,17 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="I63" s="84" t="s">
+      <c r="I63" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="J63" s="49"/>
+      <c r="J63" s="87"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="52"/>
+      <c r="A64" s="65"/>
       <c r="B64" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="53"/>
+      <c r="C64" s="66"/>
       <c r="D64" s="20" t="s">
         <v>36</v>
       </c>
@@ -3113,17 +3189,17 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="I64" s="84" t="s">
+      <c r="I64" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="J64" s="49"/>
+      <c r="J64" s="87"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="52"/>
+      <c r="A65" s="65"/>
       <c r="B65" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="53"/>
+      <c r="C65" s="66"/>
       <c r="D65" s="20" t="s">
         <v>38</v>
       </c>
@@ -3138,10 +3214,10 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="I65" s="84" t="s">
+      <c r="I65" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="J65" s="49"/>
+      <c r="J65" s="87"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B66" s="38" t="s">
@@ -3158,12 +3234,22 @@
       </c>
       <c r="H66" s="51">
         <f>SUM(H54:H65)</f>
-        <v>12</v>
-      </c>
-      <c r="I66" s="76"/>
+        <v>8.6</v>
+      </c>
+      <c r="I66" s="55"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F69">
+        <f>SUM(H19+H33+H52+H66)</f>
+        <v>30.5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="J57:J62"/>
     <mergeCell ref="J2:J4"/>
     <mergeCell ref="A54:A65"/>
     <mergeCell ref="C54:C65"/>
@@ -3177,6 +3263,9 @@
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="J38:J45"/>
     <mergeCell ref="J35:J37"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J29"/>
+    <mergeCell ref="J54:J56"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author         : Pranjal Kumar Singh File modified  : PranjalSingh.xlsx Description    : Burnt Hours Updated
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
+++ b/TeamDetails/TasksBreakDown/PranjalSingh.xlsx
@@ -745,7 +745,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -809,8 +809,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -883,8 +897,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -988,11 +1008,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1141,15 +1176,22 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1207,11 +1249,13 @@
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1525,10 +1569,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="B57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,13 +1621,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="70">
+      <c r="C2" s="73">
         <f>SUM(F2:F18)</f>
         <v>16</v>
       </c>
@@ -1606,16 +1650,16 @@
       <c r="I2" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="64">
+      <c r="J2" s="68">
         <v>42801</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="71"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="32" t="s">
         <v>21</v>
       </c>
@@ -1635,14 +1679,14 @@
       <c r="I3" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="64"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
+      <c r="A4" s="71"/>
       <c r="B4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="71"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="32" t="s">
         <v>22</v>
       </c>
@@ -1662,14 +1706,14 @@
       <c r="I4" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="64"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="71"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="32" t="s">
         <v>23</v>
       </c>
@@ -1689,16 +1733,16 @@
       <c r="I5" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="78">
+      <c r="J5" s="81">
         <v>42832</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="71"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="32" t="s">
         <v>24</v>
       </c>
@@ -1718,14 +1762,14 @@
       <c r="I6" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="79"/>
+      <c r="J6" s="82"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="71"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="32" t="s">
         <v>25</v>
       </c>
@@ -1745,14 +1789,14 @@
       <c r="I7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="79"/>
+      <c r="J7" s="82"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="71"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="32" t="s">
         <v>26</v>
       </c>
@@ -1772,14 +1816,14 @@
       <c r="I8" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="79"/>
+      <c r="J8" s="82"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="71"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="32" t="s">
         <v>27</v>
       </c>
@@ -1799,14 +1843,14 @@
       <c r="I9" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="80"/>
+      <c r="J9" s="83"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="71"/>
+      <c r="C10" s="74"/>
       <c r="D10" s="32" t="s">
         <v>32</v>
       </c>
@@ -1826,16 +1870,16 @@
       <c r="I10" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="64">
+      <c r="J10" s="68">
         <v>42862</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="71"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="32" t="s">
         <v>34</v>
       </c>
@@ -1855,14 +1899,14 @@
       <c r="I11" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="64"/>
+      <c r="J11" s="68"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="68"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="32" t="s">
         <v>36</v>
       </c>
@@ -1882,14 +1926,14 @@
       <c r="I12" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="64"/>
+      <c r="J12" s="68"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="71"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="32" t="s">
         <v>38</v>
       </c>
@@ -1910,11 +1954,11 @@
       <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="68"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="71"/>
+      <c r="C14" s="74"/>
       <c r="D14" s="32" t="s">
         <v>44</v>
       </c>
@@ -1939,11 +1983,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="68"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="71"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="32" t="s">
         <v>45</v>
       </c>
@@ -1964,11 +2008,11 @@
       <c r="J15" s="47"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="71"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="32" t="s">
         <v>52</v>
       </c>
@@ -1989,11 +2033,11 @@
       <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="68"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="71"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="32" t="s">
         <v>53</v>
       </c>
@@ -2014,11 +2058,11 @@
       <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="69"/>
+      <c r="A18" s="72"/>
       <c r="B18" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="72"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="32" t="s">
         <v>54</v>
       </c>
@@ -2060,13 +2104,13 @@
       <c r="G20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="76" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="75">
+      <c r="C21" s="78">
         <f>SUM(F21:F32)</f>
         <v>14.5</v>
       </c>
@@ -2089,16 +2133,16 @@
       <c r="I21" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J21" s="85">
+      <c r="J21" s="88">
         <v>42801</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
+      <c r="A22" s="76"/>
       <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="75"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="40" t="s">
         <v>21</v>
       </c>
@@ -2118,14 +2162,14 @@
       <c r="I22" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J22" s="75"/>
+      <c r="J22" s="78"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
+      <c r="A23" s="76"/>
       <c r="B23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="75"/>
+      <c r="C23" s="78"/>
       <c r="D23" s="40" t="s">
         <v>22</v>
       </c>
@@ -2145,14 +2189,14 @@
       <c r="I23" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J23" s="75"/>
+      <c r="J23" s="78"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
+      <c r="A24" s="76"/>
       <c r="B24" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="75"/>
+      <c r="C24" s="78"/>
       <c r="D24" s="40" t="s">
         <v>23</v>
       </c>
@@ -2172,16 +2216,16 @@
       <c r="I24" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J24" s="85">
+      <c r="J24" s="88">
         <v>42892</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="75"/>
+      <c r="C25" s="78"/>
       <c r="D25" s="40" t="s">
         <v>24</v>
       </c>
@@ -2201,14 +2245,14 @@
       <c r="I25" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="75"/>
+      <c r="J25" s="78"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
+      <c r="A26" s="76"/>
       <c r="B26" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="75"/>
+      <c r="C26" s="78"/>
       <c r="D26" s="40" t="s">
         <v>25</v>
       </c>
@@ -2228,14 +2272,14 @@
       <c r="I26" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J26" s="75"/>
+      <c r="J26" s="78"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="73"/>
+      <c r="A27" s="76"/>
       <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="75"/>
+      <c r="C27" s="78"/>
       <c r="D27" s="40" t="s">
         <v>26</v>
       </c>
@@ -2255,14 +2299,14 @@
       <c r="I27" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J27" s="75"/>
+      <c r="J27" s="78"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
+      <c r="A28" s="76"/>
       <c r="B28" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="75"/>
+      <c r="C28" s="78"/>
       <c r="D28" s="40" t="s">
         <v>27</v>
       </c>
@@ -2282,14 +2326,14 @@
       <c r="I28" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="75"/>
+      <c r="J28" s="78"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="73"/>
+      <c r="A29" s="76"/>
       <c r="B29" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="75"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="40" t="s">
         <v>32</v>
       </c>
@@ -2309,14 +2353,14 @@
       <c r="I29" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J29" s="75"/>
+      <c r="J29" s="78"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
+      <c r="A30" s="76"/>
       <c r="B30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="75"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="40" t="s">
         <v>34</v>
       </c>
@@ -2337,11 +2381,11 @@
       <c r="J30" s="49"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
+      <c r="A31" s="76"/>
       <c r="B31" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="75"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="40" t="s">
         <v>36</v>
       </c>
@@ -2362,11 +2406,11 @@
       <c r="J31" s="49"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="74"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="75"/>
+      <c r="C32" s="78"/>
       <c r="D32" s="40" t="s">
         <v>38</v>
       </c>
@@ -2408,13 +2452,13 @@
       <c r="G34"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="79" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="77">
+      <c r="C35" s="80">
         <f>SUM(F35:F51)</f>
         <v>15.5</v>
       </c>
@@ -2437,16 +2481,16 @@
       <c r="I35" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J35" s="82">
+      <c r="J35" s="85">
         <v>42801</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
+      <c r="A36" s="79"/>
       <c r="B36" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="77"/>
+      <c r="C36" s="80"/>
       <c r="D36" s="19" t="s">
         <v>21</v>
       </c>
@@ -2466,14 +2510,14 @@
       <c r="I36" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J36" s="83"/>
+      <c r="J36" s="86"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
+      <c r="A37" s="79"/>
       <c r="B37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="77"/>
+      <c r="C37" s="80"/>
       <c r="D37" s="19" t="s">
         <v>22</v>
       </c>
@@ -2493,14 +2537,14 @@
       <c r="I37" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J37" s="84"/>
+      <c r="J37" s="87"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
+      <c r="A38" s="79"/>
       <c r="B38" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="77"/>
+      <c r="C38" s="80"/>
       <c r="D38" s="19" t="s">
         <v>23</v>
       </c>
@@ -2520,16 +2564,16 @@
       <c r="I38" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J38" s="81">
+      <c r="J38" s="84">
         <v>42862</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="76"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="77"/>
+      <c r="C39" s="80"/>
       <c r="D39" s="19" t="s">
         <v>24</v>
       </c>
@@ -2549,14 +2593,14 @@
       <c r="I39" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J39" s="81"/>
+      <c r="J39" s="84"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
+      <c r="A40" s="79"/>
       <c r="B40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="77"/>
+      <c r="C40" s="80"/>
       <c r="D40" s="19" t="s">
         <v>25</v>
       </c>
@@ -2576,14 +2620,14 @@
       <c r="I40" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J40" s="81"/>
+      <c r="J40" s="84"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="76"/>
+      <c r="A41" s="79"/>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="77"/>
+      <c r="C41" s="80"/>
       <c r="D41" s="19" t="s">
         <v>26</v>
       </c>
@@ -2603,14 +2647,14 @@
       <c r="I41" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J41" s="81"/>
+      <c r="J41" s="84"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="76"/>
+      <c r="A42" s="79"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="77"/>
+      <c r="C42" s="80"/>
       <c r="D42" s="19" t="s">
         <v>27</v>
       </c>
@@ -2630,14 +2674,14 @@
       <c r="I42" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J42" s="81"/>
+      <c r="J42" s="84"/>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="76"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="77"/>
+      <c r="C43" s="80"/>
       <c r="D43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2657,14 +2701,14 @@
       <c r="I43" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J43" s="81"/>
+      <c r="J43" s="84"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="76"/>
+      <c r="A44" s="79"/>
       <c r="B44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="77"/>
+      <c r="C44" s="80"/>
       <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
@@ -2684,14 +2728,14 @@
       <c r="I44" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J44" s="81"/>
+      <c r="J44" s="84"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="76"/>
+      <c r="A45" s="79"/>
       <c r="B45" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="77"/>
+      <c r="C45" s="80"/>
       <c r="D45" s="19" t="s">
         <v>36</v>
       </c>
@@ -2711,14 +2755,14 @@
       <c r="I45" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J45" s="81"/>
+      <c r="J45" s="84"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="76"/>
+      <c r="A46" s="79"/>
       <c r="B46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="77"/>
+      <c r="C46" s="80"/>
       <c r="D46" s="19" t="s">
         <v>38</v>
       </c>
@@ -2739,11 +2783,11 @@
       <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="76"/>
+      <c r="A47" s="79"/>
       <c r="B47" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="77"/>
+      <c r="C47" s="80"/>
       <c r="D47" s="19" t="s">
         <v>44</v>
       </c>
@@ -2768,11 +2812,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
+      <c r="A48" s="79"/>
       <c r="B48" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="77"/>
+      <c r="C48" s="80"/>
       <c r="D48" s="19" t="s">
         <v>45</v>
       </c>
@@ -2793,11 +2837,11 @@
       <c r="J48" s="48"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="76"/>
+      <c r="A49" s="79"/>
       <c r="B49" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="77"/>
+      <c r="C49" s="80"/>
       <c r="D49" s="19" t="s">
         <v>52</v>
       </c>
@@ -2818,11 +2862,11 @@
       <c r="J49" s="48"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="76"/>
+      <c r="A50" s="79"/>
       <c r="B50" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="77"/>
+      <c r="C50" s="80"/>
       <c r="D50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2843,11 +2887,11 @@
       <c r="J50" s="48"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="76"/>
+      <c r="A51" s="79"/>
       <c r="B51" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="77"/>
+      <c r="C51" s="80"/>
       <c r="D51" s="19" t="s">
         <v>54</v>
       </c>
@@ -2893,13 +2937,13 @@
       <c r="I53" s="55"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="65" t="s">
+      <c r="A54" s="69" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="66">
+      <c r="C54" s="67">
         <f>SUM(F54:F65)</f>
         <v>14.5</v>
       </c>
@@ -2919,19 +2963,19 @@
         <f>F54-G54</f>
         <v>0</v>
       </c>
-      <c r="I54" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J54" s="86">
+      <c r="I54" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J54" s="66">
         <v>42801</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="65"/>
+      <c r="A55" s="69"/>
       <c r="B55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="66"/>
+      <c r="C55" s="67"/>
       <c r="D55" s="20" t="s">
         <v>21</v>
       </c>
@@ -2948,17 +2992,17 @@
         <f>F55-G55</f>
         <v>0</v>
       </c>
-      <c r="I55" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J55" s="66"/>
+      <c r="I55" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J55" s="67"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="65"/>
+      <c r="A56" s="69"/>
       <c r="B56" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="66"/>
+      <c r="C56" s="67"/>
       <c r="D56" s="20" t="s">
         <v>22</v>
       </c>
@@ -2975,17 +3019,17 @@
         <f>F56-G56</f>
         <v>0</v>
       </c>
-      <c r="I56" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J56" s="66"/>
+      <c r="I56" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J56" s="67"/>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
+      <c r="A57" s="69"/>
       <c r="B57" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="66"/>
+      <c r="C57" s="67"/>
       <c r="D57" s="20" t="s">
         <v>23</v>
       </c>
@@ -3002,19 +3046,19 @@
         <f t="shared" ref="H57:H65" si="5">F57-G57</f>
         <v>0</v>
       </c>
-      <c r="I57" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J57" s="86">
+      <c r="I57" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J57" s="66">
         <v>42892</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="65"/>
+      <c r="A58" s="69"/>
       <c r="B58" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="66"/>
+      <c r="C58" s="67"/>
       <c r="D58" s="20" t="s">
         <v>24</v>
       </c>
@@ -3031,17 +3075,17 @@
         <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
-      <c r="I58" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J58" s="66"/>
+      <c r="I58" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J58" s="67"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
+      <c r="A59" s="69"/>
       <c r="B59" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="66"/>
+      <c r="C59" s="67"/>
       <c r="D59" s="20" t="s">
         <v>25</v>
       </c>
@@ -3058,17 +3102,17 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="I59" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J59" s="66"/>
+      <c r="I59" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J59" s="67"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
+      <c r="A60" s="69"/>
       <c r="B60" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="66"/>
+      <c r="C60" s="67"/>
       <c r="D60" s="20" t="s">
         <v>26</v>
       </c>
@@ -3085,17 +3129,17 @@
         <f t="shared" si="5"/>
         <v>1.9</v>
       </c>
-      <c r="I60" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J60" s="66"/>
+      <c r="I60" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="67"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="65"/>
+      <c r="A61" s="69"/>
       <c r="B61" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="66"/>
+      <c r="C61" s="67"/>
       <c r="D61" s="20" t="s">
         <v>27</v>
       </c>
@@ -3112,17 +3156,17 @@
         <f t="shared" si="5"/>
         <v>1.9</v>
       </c>
-      <c r="I61" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J61" s="66"/>
+      <c r="I61" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61" s="67"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
+      <c r="A62" s="69"/>
       <c r="B62" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="66"/>
+      <c r="C62" s="67"/>
       <c r="D62" s="20" t="s">
         <v>32</v>
       </c>
@@ -3139,17 +3183,17 @@
         <f t="shared" si="5"/>
         <v>1.9</v>
       </c>
-      <c r="I62" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="J62" s="66"/>
+      <c r="I62" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J62" s="67"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
+      <c r="A63" s="69"/>
       <c r="B63" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="66"/>
+      <c r="C63" s="67"/>
       <c r="D63" s="20" t="s">
         <v>34</v>
       </c>
@@ -3167,14 +3211,14 @@
       <c r="I63" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="J63" s="87"/>
+      <c r="J63" s="64"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
+      <c r="A64" s="69"/>
       <c r="B64" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="66"/>
+      <c r="C64" s="67"/>
       <c r="D64" s="20" t="s">
         <v>36</v>
       </c>
@@ -3192,14 +3236,14 @@
       <c r="I64" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="J64" s="87"/>
+      <c r="J64" s="64"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
+      <c r="A65" s="69"/>
       <c r="B65" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="66"/>
+      <c r="C65" s="67"/>
       <c r="D65" s="20" t="s">
         <v>38</v>
       </c>
@@ -3217,7 +3261,7 @@
       <c r="I65" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="J65" s="87"/>
+      <c r="J65" s="64"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B66" s="38" t="s">
@@ -3238,17 +3282,26 @@
       </c>
       <c r="I66" s="55"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E69" s="1" t="s">
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E69" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="91">
         <f>SUM(H19+H33+H52+H66)</f>
         <v>30.5</v>
       </c>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E70" s="89"/>
+      <c r="F70" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="J54:J56"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
     <mergeCell ref="J57:J62"/>
     <mergeCell ref="J2:J4"/>
     <mergeCell ref="A54:A65"/>
@@ -3265,7 +3318,6 @@
     <mergeCell ref="J35:J37"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="J24:J29"/>
-    <mergeCell ref="J54:J56"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.3" footer="0.3"/>

</xml_diff>